<commit_message>
add baptismal & death template
</commit_message>
<xml_diff>
--- a/src/data/confirmation-test.xlsx
+++ b/src/data/confirmation-test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>page</t>
   </si>
@@ -22,6 +22,9 @@
     <t>no</t>
   </si>
   <si>
+    <t>date</t>
+  </si>
+  <si>
     <t>name</t>
   </si>
   <si>
@@ -31,13 +34,25 @@
     <t>mother</t>
   </si>
   <si>
-    <t>date yyyy/mm/dd</t>
-  </si>
-  <si>
     <t>priest</t>
   </si>
   <si>
-    <t>date</t>
+    <t>2017-05-24</t>
+  </si>
+  <si>
+    <t>2017-05-25</t>
+  </si>
+  <si>
+    <t>2017-05-26</t>
+  </si>
+  <si>
+    <t>2017-05-27</t>
+  </si>
+  <si>
+    <t>2017-05-28</t>
+  </si>
+  <si>
+    <t>2017-05-29</t>
   </si>
 </sst>
 </file>
@@ -45,10 +60,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -74,13 +89,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -90,7 +98,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -104,6 +120,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -112,16 +136,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -134,40 +188,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -179,25 +211,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -212,187 +227,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,16 +461,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -467,6 +482,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -488,162 +518,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -653,8 +668,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -979,12 +997,12 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C1" sqref="C$1:C$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="6"/>
   <cols>
-    <col min="6" max="6" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="17.375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -994,7 +1012,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -1017,8 +1035,8 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1027,7 +1045,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -1040,8 +1058,8 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>2</v>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>3</v>
@@ -1050,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -1063,8 +1081,8 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -1073,7 +1091,7 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G4" t="s">
         <v>6</v>
@@ -1086,8 +1104,8 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>2</v>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>3</v>
@@ -1096,7 +1114,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G5" t="s">
         <v>6</v>
@@ -1109,8 +1127,8 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
-        <v>2</v>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -1119,7 +1137,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
         <v>6</v>
@@ -1132,8 +1150,8 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>2</v>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -1142,7 +1160,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
         <v>6</v>

</xml_diff>